<commit_message>
week 39 add scatter_map to app.py
</commit_message>
<xml_diff>
--- a/Week_39_Montreal_Bicycle_Traffic/df_locations.xlsx
+++ b/Week_39_Montreal_Bicycle_Traffic/df_locations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/acb440cf5b4acec9/Programming/Plotly_FF_2025/Week_39_Montreal_Bicycle_Traffic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="149" documentId="8_{CD56B279-7348-463A-851C-574876B94837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ACFB2C91-3684-4961-A3F8-DA2532922F60}"/>
+  <xr:revisionPtr revIDLastSave="153" documentId="8_{CD56B279-7348-463A-851C-574876B94837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{243DB074-4391-4947-AA94-B030C2782E0A}"/>
   <bookViews>
-    <workbookView xWindow="6120" yWindow="3300" windowWidth="30795" windowHeight="11295" xr2:uid="{A571BB00-C5BD-49A4-B476-3DA233D3272B}"/>
+    <workbookView xWindow="7110" yWindow="2025" windowWidth="26250" windowHeight="13380" xr2:uid="{A571BB00-C5BD-49A4-B476-3DA233D3272B}"/>
   </bookViews>
   <sheets>
     <sheet name="df_locations" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="86">
   <si>
     <t>ID</t>
   </si>
@@ -169,9 +169,6 @@
     <t>Rue Saint-Denis, Ave Duluth</t>
   </si>
   <si>
-    <t>Ma Poule Mouillée (Excellent Chicken)</t>
-  </si>
-  <si>
     <t>Greenpeace Canada</t>
   </si>
   <si>
@@ -278,6 +275,12 @@
   </si>
   <si>
     <t>Route 138</t>
+  </si>
+  <si>
+    <t>Ma Poule Mouillée (Best Chicken)</t>
+  </si>
+  <si>
+    <t>Jean-Talon Market</t>
   </si>
 </sst>
 </file>
@@ -1206,8 +1209,8 @@
   <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D51" sqref="D51"/>
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1216,7 +1219,7 @@
     <col min="2" max="2" width="15.28515625" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" customWidth="1"/>
     <col min="4" max="4" width="65.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1230,7 +1233,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E1" t="s">
         <v>20</v>
@@ -1584,7 +1587,7 @@
         <v>9</v>
       </c>
       <c r="E22" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1598,10 +1601,10 @@
         <v>-73.588831449978002</v>
       </c>
       <c r="D23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1618,7 +1621,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1669,7 +1672,7 @@
         <v>13</v>
       </c>
       <c r="E27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1683,7 +1686,7 @@
         <v>-73.569540000035502</v>
       </c>
       <c r="D28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E28" t="s">
         <v>45</v>
@@ -1700,10 +1703,10 @@
         <v>-73.597115074867403</v>
       </c>
       <c r="D29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1717,10 +1720,10 @@
         <v>-73.594590000009305</v>
       </c>
       <c r="D30" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E30" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1734,10 +1737,10 @@
         <v>-73.5914628998962</v>
       </c>
       <c r="D31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E31" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1751,10 +1754,10 @@
         <v>-73.5988000000212</v>
       </c>
       <c r="D32" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E32" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1768,10 +1771,10 @@
         <v>-73.616859999969805</v>
       </c>
       <c r="D33" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E33" t="s">
-        <v>59</v>
+        <v>85</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1785,10 +1788,10 @@
         <v>-73.616870000022303</v>
       </c>
       <c r="D34" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E34" t="s">
-        <v>59</v>
+        <v>85</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1819,10 +1822,10 @@
         <v>-73.616682174933999</v>
       </c>
       <c r="D36" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E36" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1853,10 +1856,10 @@
         <v>-73.618384759950203</v>
       </c>
       <c r="D38" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E38" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1870,10 +1873,10 @@
         <v>-73.6564414499923</v>
       </c>
       <c r="D39" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E39" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1887,10 +1890,10 @@
         <v>-73.655032899946505</v>
       </c>
       <c r="D40" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E40" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -1907,7 +1910,7 @@
         <v>16</v>
       </c>
       <c r="E41" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1921,10 +1924,10 @@
         <v>-73.538816209909797</v>
       </c>
       <c r="D42" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E42" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1938,10 +1941,10 @@
         <v>-73.581043226315899</v>
       </c>
       <c r="D43" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E43" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -1958,7 +1961,7 @@
         <v>17</v>
       </c>
       <c r="E44" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -1972,10 +1975,10 @@
         <v>-73.646620000012803</v>
       </c>
       <c r="D45" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E45" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -2006,10 +2009,10 @@
         <v>-73.5100050748797</v>
       </c>
       <c r="D47" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E47" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -2040,10 +2043,10 @@
         <v>-73.613369999981998</v>
       </c>
       <c r="D49" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E49" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -2057,10 +2060,10 @@
         <v>-73.542481866569801</v>
       </c>
       <c r="D50" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E50" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -2074,10 +2077,10 @@
         <v>-73.483251449991002</v>
       </c>
       <c r="D51" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E51" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>